<commit_message>
financing features of agents added
</commit_message>
<xml_diff>
--- a/run_sheets/monopoly.xlsx
+++ b/run_sheets/monopoly.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>r</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>fixed_cost</t>
+  </si>
+  <si>
+    <t>financing_period</t>
+  </si>
+  <si>
+    <t>ordering_period</t>
+  </si>
+  <si>
+    <t>delivery_period</t>
+  </si>
+  <si>
+    <t>days_between_financing</t>
   </si>
 </sst>
 </file>
@@ -393,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" activeCellId="1" sqref="L1:L1048576 M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -411,10 +423,15 @@
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="11" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="24.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -448,8 +465,20 @@
       <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -483,8 +512,14 @@
       <c r="K2" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -518,8 +553,14 @@
       <c r="K3" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="1">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -553,61 +594,67 @@
       <c r="K4" s="1">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="1">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="5"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="5"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
agent specific features for ordering and delivery added
</commit_message>
<xml_diff>
--- a/run_sheets/monopoly.xlsx
+++ b/run_sheets/monopoly.xlsx
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M1" activeCellId="1" sqref="L1:L1048576 M1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -518,6 +518,12 @@
       <c r="M2" s="1">
         <v>90</v>
       </c>
+      <c r="N2" s="1">
+        <v>5</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -559,6 +565,12 @@
       <c r="M3" s="1">
         <v>80</v>
       </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -599,6 +611,12 @@
       </c>
       <c r="M4" s="1">
         <v>70</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>